<commit_message>
Add EWT in vendor list, Displaying of RFQ, AOQ, PO served And Cancelled
</commit_message>
<xml_diff>
--- a/Vendor Profile.xlsx
+++ b/Vendor Profile.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>VENDOR PROFILE</t>
   </si>
@@ -23,43 +23,37 @@
     <t>Vendor Name:</t>
   </si>
   <si>
-    <t>A-one Industrial Sales</t>
+    <t>2GO Express</t>
   </si>
   <si>
     <t>Address:</t>
   </si>
   <si>
-    <t>Lopez Jaena St., Libertad, Bacolod</t>
+    <t>BREDCO, Port 2, Reclamation Area, Brgy. 10, Bacolod City</t>
   </si>
   <si>
     <t>Phone Number:</t>
   </si>
   <si>
-    <t>435-7383; 432-0652; 476-1127</t>
+    <t>(034) 704-1339</t>
   </si>
   <si>
     <t>Fax Number:</t>
   </si>
   <si>
-    <t>435-7383</t>
-  </si>
-  <si>
     <t>Email:</t>
   </si>
   <si>
     <t>Contact Person:</t>
   </si>
   <si>
-    <t>Ms. Miles</t>
-  </si>
-  <si>
     <t>Terms:</t>
   </si>
   <si>
     <t>Type:</t>
   </si>
   <si>
-    <t>Re-seller, Distributor</t>
+    <t>EWT(%):</t>
   </si>
   <si>
     <t>Notes:</t>
@@ -72,48 +66,6 @@
   </si>
   <si>
     <t>Brand</t>
-  </si>
-  <si>
-    <t>Generator Capacitor Discharge Ignition</t>
-  </si>
-  <si>
-    <t>Tape</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Plywood</t>
-  </si>
-  <si>
-    <t>Grinding Disc</t>
-  </si>
-  <si>
-    <t>Tyrolit</t>
-  </si>
-  <si>
-    <t>Gold Elephant</t>
-  </si>
-  <si>
-    <t>Cutting Disc</t>
-  </si>
-  <si>
-    <t>Omega</t>
-  </si>
-  <si>
-    <t>Cutting Nozzle</t>
-  </si>
-  <si>
-    <t>Wire</t>
-  </si>
-  <si>
-    <t>Gloves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soldering lead </t>
-  </si>
-  <si>
-    <t>Brand: Rubicon</t>
   </si>
 </sst>
 </file>
@@ -517,10 +469,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -563,41 +515,39 @@
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>11</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>14</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+        <v>12</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1"/>
@@ -607,7 +557,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -615,160 +565,21 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="4"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="B7:D7"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>